<commit_message>
Author        :Deepak kandpal Files Modified:DeepakKandpal.xlsx Description   :Updated story task division excel sheet
</commit_message>
<xml_diff>
--- a/TeamDetails/TasksBreakDown/DeepakKandpal.xlsx
+++ b/TeamDetails/TasksBreakDown/DeepakKandpal.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SmaltandBeryl\Margdarshak\Industry_Internship\SSDMS-v1\trunk\TeamDetails\TasksBreakDown\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\project\trunk\TeamDetails\TasksBreakDown\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="63">
   <si>
     <t>Story ID</t>
   </si>
@@ -72,39 +72,21 @@
     <t>SSDMS-39</t>
   </si>
   <si>
-    <t>putting functionality of alert box or popup box after clicking approve button</t>
-  </si>
-  <si>
-    <t>making backend files</t>
-  </si>
-  <si>
     <t>SSDMS-40</t>
   </si>
   <si>
     <t xml:space="preserve">         T1 </t>
   </si>
   <si>
-    <t xml:space="preserve">storing the row data in the database </t>
-  </si>
-  <si>
-    <t>putting check on the reject button and making it active only when comment is written</t>
-  </si>
-  <si>
     <t xml:space="preserve">         T2</t>
   </si>
   <si>
-    <t>putting functionality of popup box to ensure the choice</t>
-  </si>
-  <si>
     <t xml:space="preserve">         T3</t>
   </si>
   <si>
     <t xml:space="preserve">         T4</t>
   </si>
   <si>
-    <t>storing the data in the database</t>
-  </si>
-  <si>
     <t xml:space="preserve">         T5</t>
   </si>
   <si>
@@ -120,27 +102,9 @@
     <t xml:space="preserve">         T1</t>
   </si>
   <si>
-    <t xml:space="preserve">making table for approved application using angular UI grid </t>
-  </si>
-  <si>
-    <t>integrating frontend with the backend</t>
-  </si>
-  <si>
-    <t>fetching data from the database</t>
-  </si>
-  <si>
-    <t>populating the data in the table from database</t>
-  </si>
-  <si>
-    <t xml:space="preserve">making table for rejected application using angular UI grid </t>
-  </si>
-  <si>
     <t xml:space="preserve">         T6</t>
   </si>
   <si>
-    <t xml:space="preserve">integerating frontend with the backend </t>
-  </si>
-  <si>
     <t xml:space="preserve">         T7 </t>
   </si>
   <si>
@@ -153,12 +117,6 @@
     <t>Review by QA</t>
   </si>
   <si>
-    <t>understing the why of the story</t>
-  </si>
-  <si>
-    <t>undestanding forward and backward linkages</t>
-  </si>
-  <si>
     <t>make block diagram of the entire code journey(work-flow)</t>
   </si>
   <si>
@@ -198,19 +156,70 @@
     <t xml:space="preserve">        T2 </t>
   </si>
   <si>
-    <t xml:space="preserve">creating the database </t>
-  </si>
-  <si>
     <t>write queries in yml</t>
   </si>
   <si>
-    <t>fetching the data from the database</t>
-  </si>
-  <si>
-    <t>populating the data in the frontend table</t>
-  </si>
-  <si>
     <t>incorporate code review changes</t>
+  </si>
+  <si>
+    <t>understand the why of the story</t>
+  </si>
+  <si>
+    <t>understand forward and backward linkages</t>
+  </si>
+  <si>
+    <t xml:space="preserve">create the database </t>
+  </si>
+  <si>
+    <t>make backend files</t>
+  </si>
+  <si>
+    <t>fetch the data from the database</t>
+  </si>
+  <si>
+    <t>populate the data in the frontend table</t>
+  </si>
+  <si>
+    <t>put functionality of alert box or popup box after clicking approve button</t>
+  </si>
+  <si>
+    <t xml:space="preserve">update the row data in the database </t>
+  </si>
+  <si>
+    <t>put check on the reject button and making it active only when comment is written</t>
+  </si>
+  <si>
+    <t>put functionality of popup box to ensure the choice</t>
+  </si>
+  <si>
+    <t>update the data in the database</t>
+  </si>
+  <si>
+    <t xml:space="preserve">make table for approved application using angular UI grid </t>
+  </si>
+  <si>
+    <t>integrate frontend with the backend</t>
+  </si>
+  <si>
+    <t>fetch data from the database</t>
+  </si>
+  <si>
+    <t>populate the data in the table from database</t>
+  </si>
+  <si>
+    <t xml:space="preserve">make table for rejected application using angular UI grid </t>
+  </si>
+  <si>
+    <t xml:space="preserve">integerate frontend with the backend </t>
+  </si>
+  <si>
+    <t>SSDMS-42</t>
+  </si>
+  <si>
+    <t>store the comment in the database</t>
+  </si>
+  <si>
+    <t xml:space="preserve">         T4 </t>
   </si>
 </sst>
 </file>
@@ -318,7 +327,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -337,15 +346,39 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2954,10 +2987,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:G46"/>
+  <dimension ref="A2:G52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A38" sqref="A38:A46"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
+      <selection sqref="A1:G52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2996,17 +3029,17 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="2" t="s">
         <v>8</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>49</v>
+        <v>35</v>
       </c>
       <c r="F3" s="2"/>
       <c r="G3" s="2" t="e">
@@ -3021,7 +3054,7 @@
         <v>9</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
@@ -3037,7 +3070,7 @@
         <v>10</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>42</v>
+        <v>28</v>
       </c>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
@@ -3053,7 +3086,7 @@
         <v>11</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
@@ -3066,10 +3099,10 @@
       <c r="A7" s="8"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>44</v>
+        <v>30</v>
       </c>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
@@ -3082,10 +3115,10 @@
       <c r="A8" s="8"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>46</v>
+        <v>32</v>
       </c>
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
@@ -3098,10 +3131,10 @@
       <c r="A9" s="8"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2" t="s">
-        <v>47</v>
+        <v>33</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>59</v>
+        <v>42</v>
       </c>
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
@@ -3114,10 +3147,10 @@
       <c r="A10" s="9"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2" t="s">
-        <v>51</v>
+        <v>37</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
@@ -3154,14 +3187,14 @@
       <c r="A13" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B13" s="2">
+      <c r="B13" s="7">
         <v>5</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>8</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="E13" s="2">
         <v>1</v>
@@ -3174,12 +3207,12 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="8"/>
-      <c r="B14" s="2"/>
+      <c r="B14" s="8"/>
       <c r="C14" s="2" t="s">
         <v>9</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>56</v>
+        <v>41</v>
       </c>
       <c r="E14" s="2">
         <v>1</v>
@@ -3192,12 +3225,12 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="8"/>
-      <c r="B15" s="2"/>
+      <c r="B15" s="8"/>
       <c r="C15" s="2" t="s">
         <v>10</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>14</v>
+        <v>46</v>
       </c>
       <c r="E15" s="2">
         <v>1</v>
@@ -3210,12 +3243,12 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="8"/>
-      <c r="B16" s="2"/>
+      <c r="B16" s="8"/>
       <c r="C16" s="2" t="s">
         <v>11</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="E16" s="2">
         <v>1</v>
@@ -3228,12 +3261,12 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="8"/>
-      <c r="B17" s="2"/>
+      <c r="B17" s="8"/>
       <c r="C17" s="2" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="E17" s="2">
         <v>1</v>
@@ -3245,13 +3278,13 @@
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="8"/>
-      <c r="B18" s="2"/>
+      <c r="A18" s="9"/>
+      <c r="B18" s="9"/>
       <c r="C18" s="2" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
@@ -3261,10 +3294,10 @@
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="8"/>
+      <c r="A19" s="2"/>
       <c r="B19" s="2"/>
       <c r="C19" s="2" t="s">
-        <v>49</v>
+        <v>35</v>
       </c>
       <c r="D19" s="3"/>
       <c r="E19" s="2"/>
@@ -3275,7 +3308,7 @@
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="8"/>
+      <c r="A20" s="2"/>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
       <c r="D20" s="3"/>
@@ -3287,7 +3320,7 @@
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="9"/>
+      <c r="A21" s="2"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
       <c r="D21" s="3"/>
@@ -3298,18 +3331,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B22" s="2">
+      <c r="B22" s="10">
         <v>6</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>8</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>13</v>
+        <v>49</v>
       </c>
       <c r="E22" s="2">
         <v>2</v>
@@ -3322,12 +3355,12 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="8"/>
-      <c r="B23" s="2"/>
+      <c r="B23" s="11"/>
       <c r="C23" s="2" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>14</v>
+        <v>46</v>
       </c>
       <c r="E23" s="2">
         <v>2</v>
@@ -3340,12 +3373,12 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="8"/>
-      <c r="B24" s="2"/>
+      <c r="B24" s="11"/>
       <c r="C24" s="2" t="s">
         <v>10</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>17</v>
+        <v>50</v>
       </c>
       <c r="E24" s="2">
         <v>2</v>
@@ -3357,13 +3390,13 @@
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="8"/>
-      <c r="B25" s="2"/>
+      <c r="A25" s="9"/>
+      <c r="B25" s="12"/>
       <c r="C25" s="2" t="s">
         <v>11</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="E25" s="2"/>
       <c r="F25" s="2"/>
@@ -3376,7 +3409,7 @@
       <c r="A26" s="2"/>
       <c r="B26" s="2"/>
       <c r="C26" s="2" t="s">
-        <v>49</v>
+        <v>35</v>
       </c>
       <c r="D26" s="3"/>
       <c r="E26" s="2"/>
@@ -3390,7 +3423,7 @@
       <c r="A27" s="2"/>
       <c r="B27" s="2"/>
       <c r="C27" s="2" t="s">
-        <v>49</v>
+        <v>35</v>
       </c>
       <c r="D27" s="3"/>
       <c r="E27" s="2"/>
@@ -3404,10 +3437,10 @@
       <c r="A28" s="2"/>
       <c r="B28" s="2"/>
       <c r="C28" s="2" t="s">
-        <v>50</v>
+        <v>36</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>48</v>
+        <v>34</v>
       </c>
       <c r="E28" s="2"/>
       <c r="F28" s="2"/>
@@ -3417,7 +3450,7 @@
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="10"/>
+      <c r="A29" s="2"/>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
       <c r="D29" s="3"/>
@@ -3430,16 +3463,16 @@
     </row>
     <row r="30" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="B30" s="2">
+        <v>13</v>
+      </c>
+      <c r="B30" s="7">
         <v>12</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D30" s="6" t="s">
-        <v>18</v>
+        <v>51</v>
       </c>
       <c r="E30" s="2">
         <v>3</v>
@@ -3452,12 +3485,12 @@
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="8"/>
-      <c r="B31" s="2"/>
+      <c r="B31" s="8"/>
       <c r="C31" s="2" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="D31" s="6" t="s">
-        <v>20</v>
+        <v>52</v>
       </c>
       <c r="E31" s="2">
         <v>3</v>
@@ -3470,12 +3503,12 @@
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="8"/>
-      <c r="B32" s="2"/>
+      <c r="B32" s="8"/>
       <c r="C32" s="2" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="D32" s="6" t="s">
-        <v>14</v>
+        <v>46</v>
       </c>
       <c r="E32" s="2">
         <v>3</v>
@@ -3488,12 +3521,12 @@
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="8"/>
-      <c r="B33" s="2"/>
+      <c r="B33" s="8"/>
       <c r="C33" s="2" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="D33" s="6" t="s">
-        <v>23</v>
+        <v>53</v>
       </c>
       <c r="E33" s="2">
         <v>3</v>
@@ -3506,12 +3539,12 @@
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="9"/>
-      <c r="B34" s="2"/>
+      <c r="B34" s="9"/>
       <c r="C34" s="2" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="D34" s="6" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="E34" s="2"/>
       <c r="F34" s="2"/>
@@ -3558,16 +3591,16 @@
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="B38" s="2">
+        <v>21</v>
+      </c>
+      <c r="B38" s="7">
         <v>17</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="D38" s="6" t="s">
-        <v>29</v>
+        <v>54</v>
       </c>
       <c r="E38" s="2">
         <v>3</v>
@@ -3580,12 +3613,12 @@
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="8"/>
-      <c r="B39" s="2"/>
+      <c r="B39" s="8"/>
       <c r="C39" s="2" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="D39" s="6" t="s">
-        <v>30</v>
+        <v>55</v>
       </c>
       <c r="E39" s="2">
         <v>2</v>
@@ -3598,12 +3631,12 @@
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="8"/>
-      <c r="B40" s="2"/>
+      <c r="B40" s="8"/>
       <c r="C40" s="2" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="D40" s="6" t="s">
-        <v>31</v>
+        <v>56</v>
       </c>
       <c r="E40" s="2">
         <v>2</v>
@@ -3616,12 +3649,12 @@
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="8"/>
-      <c r="B41" s="2"/>
+      <c r="B41" s="8"/>
       <c r="C41" s="2" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="D41" s="6" t="s">
-        <v>32</v>
+        <v>57</v>
       </c>
       <c r="E41" s="2">
         <v>2</v>
@@ -3634,12 +3667,12 @@
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="8"/>
-      <c r="B42" s="2"/>
+      <c r="B42" s="8"/>
       <c r="C42" s="2" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="D42" s="6" t="s">
-        <v>33</v>
+        <v>58</v>
       </c>
       <c r="E42" s="2">
         <v>2</v>
@@ -3652,12 +3685,12 @@
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="8"/>
-      <c r="B43" s="2"/>
+      <c r="B43" s="8"/>
       <c r="C43" s="2" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="D43" s="6" t="s">
-        <v>35</v>
+        <v>59</v>
       </c>
       <c r="E43" s="2">
         <v>2</v>
@@ -3670,12 +3703,12 @@
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="8"/>
-      <c r="B44" s="2"/>
+      <c r="B44" s="8"/>
       <c r="C44" s="2" t="s">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="D44" s="6" t="s">
-        <v>31</v>
+        <v>56</v>
       </c>
       <c r="E44" s="2">
         <v>2</v>
@@ -3688,12 +3721,12 @@
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="8"/>
-      <c r="B45" s="2"/>
+      <c r="B45" s="8"/>
       <c r="C45" s="2" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="D45" s="6" t="s">
-        <v>32</v>
+        <v>57</v>
       </c>
       <c r="E45" s="2">
         <v>2</v>
@@ -3706,12 +3739,12 @@
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="9"/>
-      <c r="B46" s="2"/>
+      <c r="B46" s="9"/>
       <c r="C46" s="2" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="D46" s="6" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="E46" s="2"/>
       <c r="F46" s="2"/>
@@ -3720,13 +3753,105 @@
         <v>0</v>
       </c>
     </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A47" s="13"/>
+      <c r="B47" s="13"/>
+      <c r="C47" s="13"/>
+      <c r="D47" s="14"/>
+      <c r="E47" s="13"/>
+      <c r="F47" s="13"/>
+      <c r="G47" s="13"/>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A48" s="13"/>
+      <c r="B48" s="13"/>
+      <c r="C48" s="13"/>
+      <c r="D48" s="14"/>
+      <c r="E48" s="13"/>
+      <c r="F48" s="13"/>
+      <c r="G48" s="13"/>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A49" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="B49" s="15">
+        <v>6</v>
+      </c>
+      <c r="C49" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="D49" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="E49" s="13">
+        <v>2</v>
+      </c>
+      <c r="F49" s="13"/>
+      <c r="G49" s="13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A50" s="17"/>
+      <c r="B50" s="17"/>
+      <c r="C50" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="D50" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="E50" s="13">
+        <v>2</v>
+      </c>
+      <c r="F50" s="13"/>
+      <c r="G50" s="13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A51" s="17"/>
+      <c r="B51" s="17"/>
+      <c r="C51" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="D51" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="E51" s="13">
+        <v>2</v>
+      </c>
+      <c r="F51" s="13"/>
+      <c r="G51" s="13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A52" s="18"/>
+      <c r="B52" s="18"/>
+      <c r="C52" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D52" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="E52" s="2"/>
+      <c r="F52" s="2"/>
+      <c r="G52" s="2"/>
+    </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="11">
+    <mergeCell ref="B13:B18"/>
+    <mergeCell ref="B22:B25"/>
+    <mergeCell ref="B30:B34"/>
+    <mergeCell ref="B38:B46"/>
+    <mergeCell ref="A49:A52"/>
+    <mergeCell ref="B49:B52"/>
     <mergeCell ref="A3:A10"/>
-    <mergeCell ref="A13:A21"/>
     <mergeCell ref="A30:A34"/>
     <mergeCell ref="A22:A25"/>
     <mergeCell ref="A38:A46"/>
+    <mergeCell ref="A13:A18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Author         : Deepak kandpal Files modified : DeepakKandpal.xlsx Description    : updated story task division excel sheet
</commit_message>
<xml_diff>
--- a/TeamDetails/TasksBreakDown/DeepakKandpal.xlsx
+++ b/TeamDetails/TasksBreakDown/DeepakKandpal.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="64">
   <si>
     <t>Story ID</t>
   </si>
@@ -156,9 +156,6 @@
     <t xml:space="preserve">        T2 </t>
   </si>
   <si>
-    <t>write queries in yml</t>
-  </si>
-  <si>
     <t>incorporate code review changes</t>
   </si>
   <si>
@@ -168,24 +165,9 @@
     <t>understand forward and backward linkages</t>
   </si>
   <si>
-    <t xml:space="preserve">create the database </t>
-  </si>
-  <si>
-    <t>make backend files</t>
-  </si>
-  <si>
-    <t>fetch the data from the database</t>
-  </si>
-  <si>
-    <t>populate the data in the frontend table</t>
-  </si>
-  <si>
     <t>put functionality of alert box or popup box after clicking approve button</t>
   </si>
   <si>
-    <t xml:space="preserve">update the row data in the database </t>
-  </si>
-  <si>
     <t>put check on the reject button and making it active only when comment is written</t>
   </si>
   <si>
@@ -216,10 +198,31 @@
     <t>SSDMS-42</t>
   </si>
   <si>
-    <t>store the comment in the database</t>
-  </si>
-  <si>
     <t xml:space="preserve">         T4 </t>
+  </si>
+  <si>
+    <t>STORY ID</t>
+  </si>
+  <si>
+    <t>connect to  database</t>
+  </si>
+  <si>
+    <t>write sql queries to fetch data from table in database</t>
+  </si>
+  <si>
+    <t>receive response from SQL</t>
+  </si>
+  <si>
+    <t>send response to frontend</t>
+  </si>
+  <si>
+    <t>update the data in database</t>
+  </si>
+  <si>
+    <t xml:space="preserve">receive response from SQL </t>
+  </si>
+  <si>
+    <t>store the comment in database</t>
   </si>
 </sst>
 </file>
@@ -243,7 +246,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -259,6 +262,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -327,7 +336,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -345,6 +354,13 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -354,30 +370,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2987,10 +2991,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:G52"/>
+  <dimension ref="A2:G55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:G52"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D59" sqref="D59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3027,82 +3031,73 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2" t="e">
-        <f>E3-F3</f>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="8"/>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2">
-        <f t="shared" ref="G4:G46" si="0">E4-F4</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="8"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E5" s="2"/>
+        <v>8</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>35</v>
+      </c>
       <c r="F5" s="2"/>
-      <c r="G5" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
+      <c r="G5" s="2" t="e">
+        <f>E5-F5</f>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="8"/>
+      <c r="A6" s="11"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>29</v>
+        <v>9</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>43</v>
       </c>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
       <c r="G6" s="2">
-        <f>E6-F6</f>
+        <f t="shared" ref="G6:G49" si="0">E6-F6</f>
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="8"/>
+      <c r="A7" s="11"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
@@ -3112,29 +3107,29 @@
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="8"/>
+      <c r="A8" s="11"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>32</v>
+        <v>11</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>29</v>
       </c>
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
       <c r="G8" s="2">
-        <f t="shared" si="0"/>
+        <f>E8-F8</f>
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="8"/>
+      <c r="A9" s="11"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2" t="s">
-        <v>33</v>
+        <v>19</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
@@ -3144,13 +3139,13 @@
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="9"/>
+      <c r="A10" s="11"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
@@ -3160,10 +3155,14 @@
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="2"/>
+      <c r="A11" s="11"/>
       <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="3"/>
+      <c r="C11" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>41</v>
+      </c>
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
       <c r="G11" s="2">
@@ -3172,10 +3171,14 @@
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="2"/>
+      <c r="A12" s="12"/>
       <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="3"/>
+      <c r="C12" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>38</v>
+      </c>
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
       <c r="G12" s="2">
@@ -3184,71 +3187,50 @@
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B13" s="7">
-        <v>5</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D13" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="E13" s="2">
-        <v>1</v>
-      </c>
+      <c r="A13" s="2"/>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="2"/>
       <c r="F13" s="2"/>
       <c r="G13" s="2">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="8"/>
-      <c r="B14" s="8"/>
-      <c r="C14" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D14" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="E14" s="2">
-        <v>1</v>
-      </c>
+      <c r="A14" s="2"/>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="2"/>
       <c r="F14" s="2"/>
       <c r="G14" s="2">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="8"/>
-      <c r="B15" s="8"/>
-      <c r="C15" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D15" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="E15" s="2">
-        <v>1</v>
-      </c>
+      <c r="A15" s="16"/>
+      <c r="B15" s="16"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="2"/>
       <c r="F15" s="2"/>
-      <c r="G15" s="2">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
+      <c r="G15" s="2"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="8"/>
-      <c r="B16" s="8"/>
+      <c r="A16" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B16" s="10">
+        <v>5</v>
+      </c>
       <c r="C16" s="2" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>47</v>
+        <v>57</v>
       </c>
       <c r="E16" s="2">
         <v>1</v>
@@ -3260,13 +3242,13 @@
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="8"/>
-      <c r="B17" s="8"/>
+      <c r="A17" s="11"/>
+      <c r="B17" s="11"/>
       <c r="C17" s="2" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>48</v>
+        <v>58</v>
       </c>
       <c r="E17" s="2">
         <v>1</v>
@@ -3278,40 +3260,50 @@
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="9"/>
-      <c r="B18" s="9"/>
+      <c r="A18" s="11"/>
+      <c r="B18" s="11"/>
       <c r="C18" s="2" t="s">
-        <v>31</v>
+        <v>10</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="E18" s="2"/>
+        <v>59</v>
+      </c>
+      <c r="E18" s="2">
+        <v>1</v>
+      </c>
       <c r="F18" s="2"/>
       <c r="G18" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="2"/>
-      <c r="B19" s="2"/>
+      <c r="A19" s="11"/>
+      <c r="B19" s="11"/>
       <c r="C19" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="D19" s="3"/>
-      <c r="E19" s="2"/>
+        <v>11</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="E19" s="2">
+        <v>2</v>
+      </c>
       <c r="F19" s="2"/>
       <c r="G19" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="2"/>
-      <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
-      <c r="D20" s="3"/>
+      <c r="A20" s="11"/>
+      <c r="B20" s="11"/>
+      <c r="C20" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>20</v>
+      </c>
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
       <c r="G20" s="2">
@@ -3320,10 +3312,12 @@
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="2"/>
-      <c r="B21" s="2"/>
-      <c r="C21" s="2"/>
-      <c r="D21" s="3"/>
+      <c r="A21" s="12"/>
+      <c r="B21" s="12"/>
+      <c r="C21" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D21" s="17"/>
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
       <c r="G21" s="2">
@@ -3332,128 +3326,128 @@
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B22" s="10">
-        <v>6</v>
-      </c>
+      <c r="A22" s="2"/>
+      <c r="B22" s="2"/>
       <c r="C22" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D22" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="E22" s="2">
-        <v>2</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="D22" s="3"/>
+      <c r="E22" s="2"/>
       <c r="F22" s="2"/>
       <c r="G22" s="2">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="8"/>
-      <c r="B23" s="11"/>
-      <c r="C23" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="D23" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="E23" s="2">
-        <v>2</v>
-      </c>
+      <c r="A23" s="2"/>
+      <c r="B23" s="2"/>
+      <c r="C23" s="2"/>
+      <c r="D23" s="3"/>
+      <c r="E23" s="2"/>
       <c r="F23" s="2"/>
       <c r="G23" s="2">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="8"/>
-      <c r="B24" s="11"/>
-      <c r="C24" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D24" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="E24" s="2">
-        <v>2</v>
-      </c>
+      <c r="A24" s="2"/>
+      <c r="B24" s="2"/>
+      <c r="C24" s="2"/>
+      <c r="D24" s="3"/>
+      <c r="E24" s="2"/>
       <c r="F24" s="2"/>
       <c r="G24" s="2">
         <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B25" s="10">
+        <v>7</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D25" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="E25" s="2">
         <v>2</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="9"/>
-      <c r="B25" s="12"/>
-      <c r="C25" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D25" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="E25" s="2"/>
       <c r="F25" s="2"/>
       <c r="G25" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="2"/>
-      <c r="B26" s="2"/>
+      <c r="A26" s="11"/>
+      <c r="B26" s="11"/>
       <c r="C26" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="D26" s="3"/>
-      <c r="E26" s="2"/>
+        <v>40</v>
+      </c>
+      <c r="D26" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="E26" s="2">
+        <v>2</v>
+      </c>
       <c r="F26" s="2"/>
       <c r="G26" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="2"/>
-      <c r="B27" s="2"/>
+      <c r="A27" s="11"/>
+      <c r="B27" s="11"/>
       <c r="C27" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="D27" s="3"/>
-      <c r="E27" s="2"/>
+        <v>10</v>
+      </c>
+      <c r="D27" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="E27" s="2">
+        <v>2</v>
+      </c>
       <c r="F27" s="2"/>
       <c r="G27" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="2"/>
-      <c r="B28" s="2"/>
+      <c r="A28" s="11"/>
+      <c r="B28" s="11"/>
       <c r="C28" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="D28" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="E28" s="2"/>
+        <v>11</v>
+      </c>
+      <c r="D28" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="E28" s="2">
+        <v>1</v>
+      </c>
       <c r="F28" s="2"/>
       <c r="G28" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="2"/>
-      <c r="B29" s="2"/>
-      <c r="C29" s="2"/>
-      <c r="D29" s="3"/>
+      <c r="A29" s="12"/>
+      <c r="B29" s="12"/>
+      <c r="C29" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D29" s="6" t="s">
+        <v>61</v>
+      </c>
       <c r="E29" s="2"/>
       <c r="F29" s="2"/>
       <c r="G29" s="2">
@@ -3461,72 +3455,60 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A30" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B30" s="7">
-        <v>12</v>
-      </c>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" s="2"/>
+      <c r="B30" s="2"/>
       <c r="C30" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D30" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="E30" s="2">
-        <v>3</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="D30" s="3"/>
+      <c r="E30" s="2"/>
       <c r="F30" s="2"/>
       <c r="G30" s="2">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" s="8"/>
-      <c r="B31" s="8"/>
+      <c r="A31" s="2"/>
+      <c r="B31" s="2"/>
       <c r="C31" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D31" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="E31" s="2">
-        <v>3</v>
-      </c>
+        <v>36</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E31" s="2"/>
       <c r="F31" s="2"/>
       <c r="G31" s="2">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="8"/>
-      <c r="B32" s="8"/>
-      <c r="C32" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D32" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="E32" s="2">
-        <v>3</v>
-      </c>
+      <c r="A32" s="2"/>
+      <c r="B32" s="2"/>
+      <c r="C32" s="2"/>
+      <c r="D32" s="3"/>
+      <c r="E32" s="2"/>
       <c r="F32" s="2"/>
       <c r="G32" s="2">
         <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" s="8"/>
-      <c r="B33" s="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A33" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B33" s="10">
+        <v>12</v>
+      </c>
       <c r="C33" s="2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D33" s="6" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="E33" s="2">
         <v>3</v>
@@ -3538,141 +3520,147 @@
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A34" s="9"/>
-      <c r="B34" s="9"/>
+      <c r="A34" s="11"/>
+      <c r="B34" s="11"/>
       <c r="C34" s="2" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D34" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="E34" s="2"/>
+        <v>46</v>
+      </c>
+      <c r="E34" s="2">
+        <v>3</v>
+      </c>
       <c r="F34" s="2"/>
       <c r="G34" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35" s="2"/>
-      <c r="B35" s="2"/>
-      <c r="C35" s="2"/>
-      <c r="D35" s="3"/>
-      <c r="E35" s="2"/>
+      <c r="A35" s="11"/>
+      <c r="B35" s="11"/>
+      <c r="C35" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D35" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="E35" s="2">
+        <v>2</v>
+      </c>
       <c r="F35" s="2"/>
       <c r="G35" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36" s="2"/>
-      <c r="B36" s="2"/>
-      <c r="C36" s="2"/>
-      <c r="D36" s="3"/>
-      <c r="E36" s="2"/>
+      <c r="A36" s="11"/>
+      <c r="B36" s="11"/>
+      <c r="C36" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D36" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="E36" s="2">
+        <v>2</v>
+      </c>
       <c r="F36" s="2"/>
       <c r="G36" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A37" s="2"/>
-      <c r="B37" s="2"/>
-      <c r="C37" s="2"/>
-      <c r="D37" s="3"/>
-      <c r="E37" s="2"/>
+      <c r="A37" s="11"/>
+      <c r="B37" s="11"/>
+      <c r="C37" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D37" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="E37" s="2">
+        <v>2</v>
+      </c>
       <c r="F37" s="2"/>
       <c r="G37" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A38" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="B38" s="7">
-        <v>17</v>
-      </c>
+      <c r="A38" s="12"/>
+      <c r="B38" s="12"/>
       <c r="C38" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D38" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="E38" s="2">
-        <v>3</v>
-      </c>
+        <v>47</v>
+      </c>
+      <c r="E38" s="2"/>
       <c r="F38" s="2"/>
       <c r="G38" s="2">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A39" s="8"/>
-      <c r="B39" s="8"/>
-      <c r="C39" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D39" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="E39" s="2">
-        <v>2</v>
-      </c>
+      <c r="A39" s="2"/>
+      <c r="B39" s="2"/>
+      <c r="C39" s="2"/>
+      <c r="D39" s="3"/>
+      <c r="E39" s="2"/>
       <c r="F39" s="2"/>
       <c r="G39" s="2">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A40" s="8"/>
-      <c r="B40" s="8"/>
-      <c r="C40" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D40" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="E40" s="2">
-        <v>2</v>
-      </c>
+      <c r="A40" s="2"/>
+      <c r="B40" s="2"/>
+      <c r="C40" s="2"/>
+      <c r="D40" s="3"/>
+      <c r="E40" s="2"/>
       <c r="F40" s="2"/>
       <c r="G40" s="2">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A41" s="8"/>
-      <c r="B41" s="8"/>
+      <c r="A41" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="B41" s="10">
+        <v>17</v>
+      </c>
       <c r="C41" s="2" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="D41" s="6" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E41" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F41" s="2"/>
       <c r="G41" s="2">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A42" s="8"/>
-      <c r="B42" s="8"/>
+      <c r="A42" s="11"/>
+      <c r="B42" s="11"/>
       <c r="C42" s="2" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D42" s="6" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="E42" s="2">
         <v>2</v>
@@ -3684,13 +3672,13 @@
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A43" s="8"/>
-      <c r="B43" s="8"/>
+      <c r="A43" s="11"/>
+      <c r="B43" s="11"/>
       <c r="C43" s="2" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="D43" s="6" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="E43" s="2">
         <v>2</v>
@@ -3702,13 +3690,13 @@
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A44" s="8"/>
-      <c r="B44" s="8"/>
+      <c r="A44" s="11"/>
+      <c r="B44" s="11"/>
       <c r="C44" s="2" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="D44" s="6" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="E44" s="2">
         <v>2</v>
@@ -3720,13 +3708,13 @@
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A45" s="8"/>
-      <c r="B45" s="8"/>
+      <c r="A45" s="11"/>
+      <c r="B45" s="11"/>
       <c r="C45" s="2" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="D45" s="6" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="E45" s="2">
         <v>2</v>
@@ -3738,120 +3726,178 @@
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A46" s="9"/>
-      <c r="B46" s="9"/>
+      <c r="A46" s="11"/>
+      <c r="B46" s="11"/>
       <c r="C46" s="2" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D46" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="E46" s="2"/>
+        <v>53</v>
+      </c>
+      <c r="E46" s="2">
+        <v>2</v>
+      </c>
       <c r="F46" s="2"/>
       <c r="G46" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A47" s="13"/>
-      <c r="B47" s="13"/>
-      <c r="C47" s="13"/>
-      <c r="D47" s="14"/>
-      <c r="E47" s="13"/>
-      <c r="F47" s="13"/>
-      <c r="G47" s="13"/>
+      <c r="A47" s="11"/>
+      <c r="B47" s="11"/>
+      <c r="C47" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D47" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="E47" s="2">
+        <v>2</v>
+      </c>
+      <c r="F47" s="2"/>
+      <c r="G47" s="2">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A48" s="13"/>
-      <c r="B48" s="13"/>
-      <c r="C48" s="13"/>
-      <c r="D48" s="14"/>
-      <c r="E48" s="13"/>
-      <c r="F48" s="13"/>
-      <c r="G48" s="13"/>
+      <c r="A48" s="11"/>
+      <c r="B48" s="11"/>
+      <c r="C48" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D48" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="E48" s="2">
+        <v>2</v>
+      </c>
+      <c r="F48" s="2"/>
+      <c r="G48" s="2">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A49" s="15" t="s">
-        <v>60</v>
-      </c>
-      <c r="B49" s="15">
+      <c r="A49" s="12"/>
+      <c r="B49" s="12"/>
+      <c r="C49" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D49" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="E49" s="2"/>
+      <c r="F49" s="2"/>
+      <c r="G49" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A50" s="7"/>
+      <c r="B50" s="7"/>
+      <c r="C50" s="7"/>
+      <c r="D50" s="8"/>
+      <c r="E50" s="7"/>
+      <c r="F50" s="7"/>
+      <c r="G50" s="7"/>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A51" s="7"/>
+      <c r="B51" s="7"/>
+      <c r="C51" s="7"/>
+      <c r="D51" s="8"/>
+      <c r="E51" s="7"/>
+      <c r="F51" s="7"/>
+      <c r="G51" s="7"/>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A52" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="B52" s="13">
         <v>6</v>
       </c>
-      <c r="C49" s="13" t="s">
+      <c r="C52" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="D49" s="16" t="s">
-        <v>41</v>
-      </c>
-      <c r="E49" s="13">
+      <c r="D52" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="E52" s="7">
         <v>2</v>
       </c>
-      <c r="F49" s="13"/>
-      <c r="G49" s="13">
+      <c r="F52" s="7"/>
+      <c r="G52" s="7">
         <v>2</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A50" s="17"/>
-      <c r="B50" s="17"/>
-      <c r="C50" s="13" t="s">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A53" s="14"/>
+      <c r="B53" s="14"/>
+      <c r="C53" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="D50" s="16" t="s">
-        <v>46</v>
-      </c>
-      <c r="E50" s="13">
+      <c r="D53" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="E53" s="7">
         <v>2</v>
       </c>
-      <c r="F50" s="13"/>
-      <c r="G50" s="13">
+      <c r="F53" s="7"/>
+      <c r="G53" s="7">
         <v>2</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A51" s="17"/>
-      <c r="B51" s="17"/>
-      <c r="C51" s="13" t="s">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A54" s="14"/>
+      <c r="B54" s="14"/>
+      <c r="C54" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="D51" s="16" t="s">
-        <v>61</v>
-      </c>
-      <c r="E51" s="13">
+      <c r="D54" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="E54" s="7">
+        <v>1</v>
+      </c>
+      <c r="F54" s="7"/>
+      <c r="G54" s="7">
         <v>2</v>
       </c>
-      <c r="F51" s="13"/>
-      <c r="G51" s="13">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A52" s="18"/>
-      <c r="B52" s="18"/>
-      <c r="C52" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="D52" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="E52" s="2"/>
-      <c r="F52" s="2"/>
-      <c r="G52" s="2"/>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A55" s="15"/>
+      <c r="B55" s="15"/>
+      <c r="C55" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="D55" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="E55" s="2">
+        <v>1</v>
+      </c>
+      <c r="F55" s="2"/>
+      <c r="G55" s="2">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="B13:B18"/>
-    <mergeCell ref="B22:B25"/>
-    <mergeCell ref="B30:B34"/>
-    <mergeCell ref="B38:B46"/>
-    <mergeCell ref="A49:A52"/>
-    <mergeCell ref="B49:B52"/>
-    <mergeCell ref="A3:A10"/>
-    <mergeCell ref="A30:A34"/>
-    <mergeCell ref="A22:A25"/>
-    <mergeCell ref="A38:A46"/>
-    <mergeCell ref="A13:A18"/>
+    <mergeCell ref="A5:A12"/>
+    <mergeCell ref="A16:A21"/>
+    <mergeCell ref="A25:A29"/>
+    <mergeCell ref="A33:A38"/>
+    <mergeCell ref="A41:A49"/>
+    <mergeCell ref="B16:B21"/>
+    <mergeCell ref="B25:B29"/>
+    <mergeCell ref="B33:B38"/>
+    <mergeCell ref="B41:B49"/>
+    <mergeCell ref="A52:A55"/>
+    <mergeCell ref="B52:B55"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Author        : Deepak kandpal Files modified: DeepakKandpal.xlsx Description   : updated excel sheet 4/7/17
</commit_message>
<xml_diff>
--- a/TeamDetails/TasksBreakDown/DeepakKandpal.xlsx
+++ b/TeamDetails/TasksBreakDown/DeepakKandpal.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="4"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Name 1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="69">
   <si>
     <t>Story ID</t>
   </si>
@@ -93,9 +93,6 @@
     <t xml:space="preserve">        T5</t>
   </si>
   <si>
-    <t>review by QA</t>
-  </si>
-  <si>
     <t>SSDMS-43</t>
   </si>
   <si>
@@ -114,15 +111,6 @@
     <t xml:space="preserve">         T9 </t>
   </si>
   <si>
-    <t>Review by QA</t>
-  </si>
-  <si>
-    <t>make block diagram of the entire code journey(work-flow)</t>
-  </si>
-  <si>
-    <t>technical understanding</t>
-  </si>
-  <si>
     <t>unit testing</t>
   </si>
   <si>
@@ -159,12 +147,6 @@
     <t>incorporate code review changes</t>
   </si>
   <si>
-    <t>understand the why of the story</t>
-  </si>
-  <si>
-    <t>understand forward and backward linkages</t>
-  </si>
-  <si>
     <t>put functionality of alert box or popup box after clicking approve button</t>
   </si>
   <si>
@@ -223,6 +205,39 @@
   </si>
   <si>
     <t>store the comment in database</t>
+  </si>
+  <si>
+    <t>Understand the why of the story</t>
+  </si>
+  <si>
+    <t>Understand forward and backward linkages</t>
+  </si>
+  <si>
+    <t>Make block diagram of the entire code journey(work-flow)</t>
+  </si>
+  <si>
+    <t>Develop technical understanding</t>
+  </si>
+  <si>
+    <t>Review and Incoporate feedback</t>
+  </si>
+  <si>
+    <t>code refactoring</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            </t>
+  </si>
+  <si>
+    <t>putting validation on edit button</t>
+  </si>
+  <si>
+    <t xml:space="preserve">         T8</t>
+  </si>
+  <si>
+    <t>sending comment to the controller</t>
+  </si>
+  <si>
+    <t>review and incorporate feedback</t>
   </si>
 </sst>
 </file>
@@ -336,7 +351,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -361,6 +376,11 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -378,10 +398,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2991,10 +3007,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:G55"/>
+  <dimension ref="A2:G58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D59" sqref="D59"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E61" sqref="E61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3033,7 +3049,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>6</v>
@@ -3055,65 +3071,62 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="10" t="s">
-        <v>39</v>
+      <c r="A5" s="13" t="s">
+        <v>35</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" s="2" t="s">
         <v>8</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>42</v>
+        <v>58</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="F5" s="2"/>
-      <c r="G5" s="2" t="e">
-        <f>E5-F5</f>
-        <v>#VALUE!</v>
-      </c>
+      <c r="G5" s="2"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="11"/>
+      <c r="A6" s="14"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2" t="s">
         <v>9</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>43</v>
+        <v>59</v>
       </c>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
       <c r="G6" s="2">
-        <f t="shared" ref="G6:G49" si="0">E6-F6</f>
+        <f>E6-H9</f>
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="11"/>
+      <c r="A7" s="14"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2" t="s">
         <v>10</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>28</v>
+        <v>60</v>
       </c>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
       <c r="G7" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="G7:G49" si="0">E7-F7</f>
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="11"/>
+      <c r="A8" s="14"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2" t="s">
         <v>11</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>29</v>
+        <v>61</v>
       </c>
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
@@ -3123,29 +3136,29 @@
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="11"/>
+      <c r="A9" s="14"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2" t="s">
         <v>19</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
       <c r="G9" s="2">
-        <f t="shared" si="0"/>
+        <f>E9-F9</f>
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="11"/>
+      <c r="A10" s="14"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
@@ -3155,13 +3168,13 @@
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="11"/>
+      <c r="A11" s="14"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
@@ -3171,13 +3184,13 @@
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="12"/>
+      <c r="A12" s="15"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
@@ -3211,26 +3224,36 @@
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="16"/>
-      <c r="B15" s="16"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
-      <c r="G15" s="2"/>
+      <c r="A15" s="10"/>
+      <c r="B15" s="13">
+        <v>8</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="E15" s="2">
+        <v>2</v>
+      </c>
+      <c r="F15" s="2">
+        <v>1.5</v>
+      </c>
+      <c r="G15" s="2">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="10" t="s">
+      <c r="A16" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="10">
-        <v>5</v>
-      </c>
+      <c r="B16" s="14"/>
       <c r="C16" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="E16" s="2">
         <v>1</v>
@@ -3242,31 +3265,33 @@
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="11"/>
-      <c r="B17" s="11"/>
+      <c r="A17" s="14"/>
+      <c r="B17" s="14"/>
       <c r="C17" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="E17" s="2">
         <v>1</v>
       </c>
-      <c r="F17" s="2"/>
+      <c r="F17" s="2">
+        <v>0.5</v>
+      </c>
       <c r="G17" s="2">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="11"/>
-      <c r="B18" s="11"/>
+      <c r="A18" s="14"/>
+      <c r="B18" s="14"/>
       <c r="C18" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="E18" s="2">
         <v>1</v>
@@ -3278,13 +3303,13 @@
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="11"/>
-      <c r="B19" s="11"/>
+      <c r="A19" s="14"/>
+      <c r="B19" s="14"/>
       <c r="C19" s="2" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="E19" s="2">
         <v>2</v>
@@ -3296,28 +3321,30 @@
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="11"/>
-      <c r="B20" s="11"/>
+      <c r="A20" s="14"/>
+      <c r="B20" s="14"/>
       <c r="C20" s="2" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="E20" s="2"/>
+        <v>68</v>
+      </c>
+      <c r="E20" s="2">
+        <v>1</v>
+      </c>
       <c r="F20" s="2"/>
       <c r="G20" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f>E20-F20</f>
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="12"/>
-      <c r="B21" s="12"/>
+      <c r="A21" s="15"/>
+      <c r="B21" s="15"/>
       <c r="C21" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="D21" s="17"/>
+        <v>32</v>
+      </c>
+      <c r="D21" s="11"/>
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
       <c r="G21" s="2">
@@ -3329,7 +3356,7 @@
       <c r="A22" s="2"/>
       <c r="B22" s="2"/>
       <c r="C22" s="2" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="D22" s="3"/>
       <c r="E22" s="2"/>
@@ -3364,35 +3391,37 @@
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="10" t="s">
+      <c r="A25" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="B25" s="10">
-        <v>7</v>
+      <c r="B25" s="13">
+        <v>9</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>8</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="E25" s="2">
         <v>2</v>
       </c>
-      <c r="F25" s="2"/>
+      <c r="F25" s="2">
+        <v>1</v>
+      </c>
       <c r="G25" s="2">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="11"/>
-      <c r="B26" s="11"/>
+      <c r="A26" s="14"/>
+      <c r="B26" s="14"/>
       <c r="C26" s="2" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D26" s="6" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="E26" s="2">
         <v>2</v>
@@ -3404,31 +3433,33 @@
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="11"/>
-      <c r="B27" s="11"/>
+      <c r="A27" s="14"/>
+      <c r="B27" s="14"/>
       <c r="C27" s="2" t="s">
         <v>10</v>
       </c>
       <c r="D27" s="6" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="E27" s="2">
         <v>2</v>
       </c>
-      <c r="F27" s="2"/>
+      <c r="F27" s="2">
+        <v>0.5</v>
+      </c>
       <c r="G27" s="2">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="11"/>
-      <c r="B28" s="11"/>
+      <c r="A28" s="14"/>
+      <c r="B28" s="14"/>
       <c r="C28" s="2" t="s">
         <v>11</v>
       </c>
       <c r="D28" s="6" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="E28" s="2">
         <v>1</v>
@@ -3440,26 +3471,28 @@
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="12"/>
-      <c r="B29" s="12"/>
+      <c r="A29" s="15"/>
+      <c r="B29" s="15"/>
       <c r="C29" s="2" t="s">
         <v>19</v>
       </c>
       <c r="D29" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="E29" s="2"/>
+        <v>55</v>
+      </c>
+      <c r="E29" s="2">
+        <v>2</v>
+      </c>
       <c r="F29" s="2"/>
       <c r="G29" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="2"/>
       <c r="B30" s="2"/>
       <c r="C30" s="2" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="D30" s="3"/>
       <c r="E30" s="2"/>
@@ -3473,10 +3506,10 @@
       <c r="A31" s="2"/>
       <c r="B31" s="2"/>
       <c r="C31" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="E31" s="2"/>
       <c r="F31" s="2"/>
@@ -3498,17 +3531,17 @@
       </c>
     </row>
     <row r="33" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A33" s="10" t="s">
+      <c r="A33" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B33" s="10">
+      <c r="B33" s="13">
         <v>12</v>
       </c>
       <c r="C33" s="2" t="s">
         <v>14</v>
       </c>
       <c r="D33" s="6" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="E33" s="2">
         <v>3</v>
@@ -3520,13 +3553,13 @@
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A34" s="11"/>
-      <c r="B34" s="11"/>
+      <c r="A34" s="14"/>
+      <c r="B34" s="14"/>
       <c r="C34" s="2" t="s">
         <v>15</v>
       </c>
       <c r="D34" s="6" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="E34" s="2">
         <v>3</v>
@@ -3538,13 +3571,13 @@
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35" s="11"/>
-      <c r="B35" s="11"/>
+      <c r="A35" s="14"/>
+      <c r="B35" s="14"/>
       <c r="C35" s="2" t="s">
         <v>16</v>
       </c>
       <c r="D35" s="6" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="E35" s="2">
         <v>2</v>
@@ -3556,31 +3589,32 @@
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36" s="11"/>
-      <c r="B36" s="11"/>
+      <c r="A36" s="14"/>
+      <c r="B36" s="14"/>
       <c r="C36" s="2" t="s">
         <v>17</v>
       </c>
       <c r="D36" s="6" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="E36" s="2">
         <v>2</v>
       </c>
-      <c r="F36" s="2"/>
+      <c r="F36" s="2" t="s">
+        <v>64</v>
+      </c>
       <c r="G36" s="2">
-        <f t="shared" si="0"/>
         <v>2</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A37" s="11"/>
-      <c r="B37" s="11"/>
+      <c r="A37" s="14"/>
+      <c r="B37" s="14"/>
       <c r="C37" s="2" t="s">
         <v>18</v>
       </c>
       <c r="D37" s="6" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="E37" s="2">
         <v>2</v>
@@ -3592,19 +3626,21 @@
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A38" s="12"/>
-      <c r="B38" s="12"/>
+      <c r="A38" s="15"/>
+      <c r="B38" s="15"/>
       <c r="C38" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D38" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="E38" s="2"/>
+        <v>41</v>
+      </c>
+      <c r="E38" s="2">
+        <v>2</v>
+      </c>
       <c r="F38" s="2"/>
       <c r="G38" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
@@ -3615,7 +3651,7 @@
       <c r="E39" s="2"/>
       <c r="F39" s="2"/>
       <c r="G39" s="2">
-        <f t="shared" si="0"/>
+        <f>E39-F39</f>
         <v>0</v>
       </c>
     </row>
@@ -3632,17 +3668,17 @@
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A41" s="10" t="s">
+      <c r="A41" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="B41" s="13">
+        <v>17</v>
+      </c>
+      <c r="C41" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B41" s="10">
-        <v>17</v>
-      </c>
-      <c r="C41" s="2" t="s">
-        <v>22</v>
-      </c>
       <c r="D41" s="6" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="E41" s="2">
         <v>3</v>
@@ -3654,13 +3690,13 @@
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A42" s="11"/>
-      <c r="B42" s="11"/>
+      <c r="A42" s="14"/>
+      <c r="B42" s="14"/>
       <c r="C42" s="2" t="s">
         <v>15</v>
       </c>
       <c r="D42" s="6" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="E42" s="2">
         <v>2</v>
@@ -3672,13 +3708,13 @@
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A43" s="11"/>
-      <c r="B43" s="11"/>
+      <c r="A43" s="14"/>
+      <c r="B43" s="14"/>
       <c r="C43" s="2" t="s">
         <v>16</v>
       </c>
       <c r="D43" s="6" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="E43" s="2">
         <v>2</v>
@@ -3690,13 +3726,13 @@
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A44" s="11"/>
-      <c r="B44" s="11"/>
+      <c r="A44" s="14"/>
+      <c r="B44" s="14"/>
       <c r="C44" s="2" t="s">
         <v>17</v>
       </c>
       <c r="D44" s="6" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="E44" s="2">
         <v>2</v>
@@ -3708,13 +3744,13 @@
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A45" s="11"/>
-      <c r="B45" s="11"/>
+      <c r="A45" s="14"/>
+      <c r="B45" s="14"/>
       <c r="C45" s="2" t="s">
         <v>18</v>
       </c>
       <c r="D45" s="6" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="E45" s="2">
         <v>2</v>
@@ -3726,13 +3762,13 @@
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A46" s="11"/>
-      <c r="B46" s="11"/>
+      <c r="A46" s="14"/>
+      <c r="B46" s="14"/>
       <c r="C46" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D46" s="6" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="E46" s="2">
         <v>2</v>
@@ -3744,13 +3780,13 @@
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A47" s="11"/>
-      <c r="B47" s="11"/>
+      <c r="A47" s="14"/>
+      <c r="B47" s="14"/>
       <c r="C47" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D47" s="6" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="E47" s="2">
         <v>2</v>
@@ -3762,13 +3798,13 @@
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A48" s="11"/>
-      <c r="B48" s="11"/>
+      <c r="A48" s="14"/>
+      <c r="B48" s="14"/>
       <c r="C48" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D48" s="6" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="E48" s="2">
         <v>2</v>
@@ -3780,19 +3816,21 @@
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A49" s="12"/>
-      <c r="B49" s="12"/>
+      <c r="A49" s="15"/>
+      <c r="B49" s="15"/>
       <c r="C49" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D49" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="E49" s="2"/>
+        <v>62</v>
+      </c>
+      <c r="E49" s="2">
+        <v>2</v>
+      </c>
       <c r="F49" s="2"/>
       <c r="G49" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
@@ -3806,25 +3844,35 @@
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="7"/>
-      <c r="B51" s="7"/>
-      <c r="C51" s="7"/>
-      <c r="D51" s="8"/>
-      <c r="E51" s="7"/>
-      <c r="F51" s="7"/>
-      <c r="G51" s="7"/>
+      <c r="B51" s="16">
+        <v>11</v>
+      </c>
+      <c r="C51" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D51" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="E51" s="7">
+        <v>2</v>
+      </c>
+      <c r="F51" s="7">
+        <v>1.5</v>
+      </c>
+      <c r="G51" s="7">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A52" s="13" t="s">
-        <v>54</v>
-      </c>
-      <c r="B52" s="13">
-        <v>6</v>
-      </c>
+      <c r="A52" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="B52" s="17"/>
       <c r="C52" s="7" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="D52" s="9" t="s">
-        <v>57</v>
+        <v>65</v>
       </c>
       <c r="E52" s="7">
         <v>2</v>
@@ -3835,16 +3883,16 @@
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A53" s="14"/>
-      <c r="B53" s="14"/>
+      <c r="A53" s="17"/>
+      <c r="B53" s="17"/>
       <c r="C53" s="7" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D53" s="9" t="s">
-        <v>58</v>
+        <v>67</v>
       </c>
       <c r="E53" s="7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F53" s="7"/>
       <c r="G53" s="7">
@@ -3852,13 +3900,13 @@
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A54" s="14"/>
-      <c r="B54" s="14"/>
+      <c r="A54" s="17"/>
+      <c r="B54" s="17"/>
       <c r="C54" s="7" t="s">
-        <v>16</v>
+        <v>49</v>
       </c>
       <c r="D54" s="9" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="E54" s="7">
         <v>1</v>
@@ -3869,13 +3917,13 @@
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A55" s="15"/>
-      <c r="B55" s="15"/>
+      <c r="A55" s="17"/>
+      <c r="B55" s="17"/>
       <c r="C55" s="2" t="s">
-        <v>55</v>
+        <v>18</v>
       </c>
       <c r="D55" s="6" t="s">
-        <v>63</v>
+        <v>52</v>
       </c>
       <c r="E55" s="2">
         <v>1</v>
@@ -3885,19 +3933,68 @@
         <v>1</v>
       </c>
     </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A56" s="18"/>
+      <c r="B56" s="17"/>
+      <c r="C56" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D56" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="E56" s="12">
+        <v>2</v>
+      </c>
+      <c r="F56" s="2"/>
+      <c r="G56" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B57" s="17"/>
+      <c r="C57" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D57" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="E57" s="2">
+        <v>1</v>
+      </c>
+      <c r="F57" s="2"/>
+      <c r="G57" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B58" s="18"/>
+      <c r="C58" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="D58" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="E58" s="2">
+        <v>1</v>
+      </c>
+      <c r="F58" s="2"/>
+      <c r="G58" s="2">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="B25:B29"/>
+    <mergeCell ref="B33:B38"/>
+    <mergeCell ref="B41:B49"/>
+    <mergeCell ref="A52:A56"/>
+    <mergeCell ref="B15:B21"/>
+    <mergeCell ref="B51:B58"/>
     <mergeCell ref="A5:A12"/>
     <mergeCell ref="A16:A21"/>
     <mergeCell ref="A25:A29"/>
     <mergeCell ref="A33:A38"/>
     <mergeCell ref="A41:A49"/>
-    <mergeCell ref="B16:B21"/>
-    <mergeCell ref="B25:B29"/>
-    <mergeCell ref="B33:B38"/>
-    <mergeCell ref="B41:B49"/>
-    <mergeCell ref="A52:A55"/>
-    <mergeCell ref="B52:B55"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>